<commit_message>
add tool to trim sounds
</commit_message>
<xml_diff>
--- a/annotation_sounds.xlsx
+++ b/annotation_sounds.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="620" yWindow="520" windowWidth="25600" windowHeight="15700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -510,9 +510,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,15 +845,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C151"/>
+  <dimension ref="A1:F151"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="D151" sqref="D151"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -862,8 +863,14 @@
       <c r="C1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="F1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -873,8 +880,14 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -884,8 +897,14 @@
       <c r="C3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -895,8 +914,14 @@
       <c r="C4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="E4">
+        <v>-1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -906,8 +931,14 @@
       <c r="C5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -917,8 +948,14 @@
       <c r="C6">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="E6">
+        <v>-1</v>
+      </c>
+      <c r="F6">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -928,8 +965,14 @@
       <c r="C7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -939,8 +982,14 @@
       <c r="C8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="E8">
+        <v>-0.5</v>
+      </c>
+      <c r="F8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -950,8 +999,14 @@
       <c r="C9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -961,8 +1016,14 @@
       <c r="C10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -972,8 +1033,14 @@
       <c r="C11">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -983,8 +1050,14 @@
       <c r="C12">
         <v>-1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="E12">
+        <v>-1</v>
+      </c>
+      <c r="F12">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -994,8 +1067,14 @@
       <c r="C13">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1005,8 +1084,14 @@
       <c r="C14">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1016,8 +1101,14 @@
       <c r="C15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1027,8 +1118,14 @@
       <c r="C16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1038,8 +1135,14 @@
       <c r="C17">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="E17">
+        <v>0.5</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1049,8 +1152,14 @@
       <c r="C18">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1060,8 +1169,14 @@
       <c r="C19">
         <v>-1</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="E19">
+        <v>-1</v>
+      </c>
+      <c r="F19">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1071,8 +1186,14 @@
       <c r="C20">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="E20">
+        <v>0.5</v>
+      </c>
+      <c r="F20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1082,8 +1203,14 @@
       <c r="C21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1093,8 +1220,14 @@
       <c r="C22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="E22">
+        <v>0.5</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1104,8 +1237,14 @@
       <c r="C23">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1115,8 +1254,14 @@
       <c r="C24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="E24">
+        <v>-0.5</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1126,8 +1271,14 @@
       <c r="C25">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1137,8 +1288,14 @@
       <c r="C26">
         <v>-1</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="E26">
+        <v>-1</v>
+      </c>
+      <c r="F26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1148,8 +1305,14 @@
       <c r="C27">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="E27">
+        <v>-1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1159,8 +1322,14 @@
       <c r="C28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1170,8 +1339,14 @@
       <c r="C29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="E29">
+        <v>0.5</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1181,8 +1356,14 @@
       <c r="C30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1192,8 +1373,14 @@
       <c r="C31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1203,8 +1390,14 @@
       <c r="C32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="E32">
+        <v>0.5</v>
+      </c>
+      <c r="F32">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1214,8 +1407,14 @@
       <c r="C33">
         <v>-1</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="E33">
+        <v>-1</v>
+      </c>
+      <c r="F33">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1225,8 +1424,14 @@
       <c r="C34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="E34">
+        <v>-0.5</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1236,8 +1441,14 @@
       <c r="C35">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="E35">
+        <v>-1</v>
+      </c>
+      <c r="F35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1247,8 +1458,14 @@
       <c r="C36">
         <v>-1</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="E36">
+        <v>-1</v>
+      </c>
+      <c r="F36">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1258,8 +1475,14 @@
       <c r="C37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="E37">
+        <v>-1</v>
+      </c>
+      <c r="F37">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1269,8 +1492,14 @@
       <c r="C38">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="E38">
+        <v>0.5</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1280,8 +1509,14 @@
       <c r="C39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="E39">
+        <v>0.5</v>
+      </c>
+      <c r="F39">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1291,8 +1526,14 @@
       <c r="C40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="E40">
+        <v>0.5</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1302,8 +1543,14 @@
       <c r="C41">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1313,8 +1560,14 @@
       <c r="C42">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1324,8 +1577,14 @@
       <c r="C43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1335,8 +1594,14 @@
       <c r="C44">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="E44">
+        <v>-1</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1346,8 +1611,14 @@
       <c r="C45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="E45">
+        <v>-1</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1357,8 +1628,14 @@
       <c r="C46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1368,8 +1645,14 @@
       <c r="C47">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="E47">
+        <v>0.5</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1379,8 +1662,14 @@
       <c r="C48">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="E48">
+        <v>0.5</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1390,8 +1679,14 @@
       <c r="C49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1401,8 +1696,14 @@
       <c r="C50">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1412,8 +1713,14 @@
       <c r="C51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="E51">
+        <v>-1</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1423,8 +1730,14 @@
       <c r="C52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1434,8 +1747,14 @@
       <c r="C53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1445,8 +1764,14 @@
       <c r="C54">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="E54">
+        <v>0.5</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1456,8 +1781,14 @@
       <c r="C55">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -1467,8 +1798,14 @@
       <c r="C56">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="E56">
+        <v>0.5</v>
+      </c>
+      <c r="F56">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -1478,8 +1815,14 @@
       <c r="C57">
         <v>-1</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -1489,8 +1832,14 @@
       <c r="C58">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="59" spans="1:3">
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -1500,8 +1849,14 @@
       <c r="C59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="E59">
+        <v>0.5</v>
+      </c>
+      <c r="F59">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -1511,8 +1866,14 @@
       <c r="C60">
         <v>-1</v>
       </c>
-    </row>
-    <row r="61" spans="1:3">
+      <c r="E60">
+        <v>-1</v>
+      </c>
+      <c r="F60">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -1522,8 +1883,14 @@
       <c r="C61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -1533,8 +1900,14 @@
       <c r="C62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -1544,8 +1917,14 @@
       <c r="C63">
         <v>-1</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
+      <c r="E63">
+        <v>0.5</v>
+      </c>
+      <c r="F63">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -1555,8 +1934,14 @@
       <c r="C64">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
+      <c r="E64">
+        <v>-1</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -1566,8 +1951,14 @@
       <c r="C65">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:3">
+      <c r="E65">
+        <v>-1</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -1577,8 +1968,14 @@
       <c r="C67">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
+      <c r="E67">
+        <v>0.5</v>
+      </c>
+      <c r="F67">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -1588,8 +1985,14 @@
       <c r="C68">
         <v>-1</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
+      <c r="E68">
+        <v>0.5</v>
+      </c>
+      <c r="F68">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -1599,8 +2002,14 @@
       <c r="C69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -1610,8 +2019,14 @@
       <c r="C70">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
+      <c r="E70">
+        <v>-1</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -1621,8 +2036,14 @@
       <c r="C71">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -1632,8 +2053,14 @@
       <c r="C72">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
+      <c r="E72">
+        <v>-1</v>
+      </c>
+      <c r="F72">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -1643,8 +2070,14 @@
       <c r="C73">
         <v>-1</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="E73">
+        <v>0.5</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -1654,8 +2087,14 @@
       <c r="C74">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
+      <c r="E74">
+        <v>-0.5</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -1665,8 +2104,14 @@
       <c r="C75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:3">
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="F75">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -1676,8 +2121,14 @@
       <c r="C76">
         <v>-1</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -1687,8 +2138,14 @@
       <c r="C77">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="78" spans="1:3">
+      <c r="E77">
+        <v>0.5</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -1698,8 +2155,14 @@
       <c r="C78">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="79" spans="1:3">
+      <c r="E78">
+        <v>-1</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -1709,8 +2172,14 @@
       <c r="C79">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="80" spans="1:3">
+      <c r="E79">
+        <v>0.5</v>
+      </c>
+      <c r="F79">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -1720,8 +2189,14 @@
       <c r="C80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:3">
+      <c r="E80">
+        <v>0.5</v>
+      </c>
+      <c r="F80">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>79</v>
       </c>
@@ -1731,8 +2206,14 @@
       <c r="C81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:3">
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>80</v>
       </c>
@@ -1742,8 +2223,14 @@
       <c r="C82">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="83" spans="1:3">
+      <c r="E82">
+        <v>0.5</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
       <c r="A83" t="s">
         <v>81</v>
       </c>
@@ -1753,8 +2240,14 @@
       <c r="C83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:3">
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -1764,8 +2257,14 @@
       <c r="C84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:3">
+      <c r="E84">
+        <v>1</v>
+      </c>
+      <c r="F84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
       <c r="A85" t="s">
         <v>83</v>
       </c>
@@ -1775,8 +2274,14 @@
       <c r="C85">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="86" spans="1:3">
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
       <c r="A86" t="s">
         <v>84</v>
       </c>
@@ -1786,8 +2291,14 @@
       <c r="C86">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="87" spans="1:3">
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
       <c r="A87" s="1" t="s">
         <v>85</v>
       </c>
@@ -1797,8 +2308,14 @@
       <c r="C87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:3">
+      <c r="E87">
+        <v>-0.5</v>
+      </c>
+      <c r="F87">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
       <c r="A88" t="s">
         <v>86</v>
       </c>
@@ -1808,8 +2325,14 @@
       <c r="C88">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="89" spans="1:3">
+      <c r="E88">
+        <v>0.5</v>
+      </c>
+      <c r="F88">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -1819,8 +2342,14 @@
       <c r="C89">
         <v>-1</v>
       </c>
-    </row>
-    <row r="90" spans="1:3">
+      <c r="E89">
+        <v>-0.5</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
       <c r="A90" t="s">
         <v>88</v>
       </c>
@@ -1830,8 +2359,14 @@
       <c r="C90">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="91" spans="1:3">
+      <c r="E90">
+        <v>-0.5</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
       <c r="A91" t="s">
         <v>89</v>
       </c>
@@ -1841,8 +2376,14 @@
       <c r="C91">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="92" spans="1:3">
+      <c r="E91">
+        <v>-0.5</v>
+      </c>
+      <c r="F91">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
       <c r="A92" t="s">
         <v>90</v>
       </c>
@@ -1852,8 +2393,14 @@
       <c r="C92">
         <v>-1</v>
       </c>
-    </row>
-    <row r="93" spans="1:3">
+      <c r="E92">
+        <v>-1</v>
+      </c>
+      <c r="F92">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -1863,8 +2410,14 @@
       <c r="C93">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="94" spans="1:3">
+      <c r="E93">
+        <v>-1</v>
+      </c>
+      <c r="F93">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -1874,8 +2427,14 @@
       <c r="C94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:3">
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
       <c r="A95" t="s">
         <v>93</v>
       </c>
@@ -1885,8 +2444,14 @@
       <c r="C95">
         <v>-1</v>
       </c>
-    </row>
-    <row r="96" spans="1:3">
+      <c r="E95">
+        <v>0.5</v>
+      </c>
+      <c r="F95">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
       <c r="A96" t="s">
         <v>94</v>
       </c>
@@ -1896,8 +2461,14 @@
       <c r="C96">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="97" spans="1:3">
+      <c r="E96">
+        <v>-1</v>
+      </c>
+      <c r="F96">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -1907,8 +2478,14 @@
       <c r="C97">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="98" spans="1:3">
+      <c r="E97">
+        <v>0.5</v>
+      </c>
+      <c r="F97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
       <c r="A98" t="s">
         <v>96</v>
       </c>
@@ -1918,8 +2495,14 @@
       <c r="C98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:3">
+      <c r="E98">
+        <v>-1</v>
+      </c>
+      <c r="F98">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -1929,8 +2512,14 @@
       <c r="C99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:3">
+      <c r="E99">
+        <v>-1</v>
+      </c>
+      <c r="F99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
       <c r="A100" t="s">
         <v>98</v>
       </c>
@@ -1940,8 +2529,14 @@
       <c r="C100">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="101" spans="1:3">
+      <c r="E100">
+        <v>0.5</v>
+      </c>
+      <c r="F100">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
       <c r="A101" t="s">
         <v>99</v>
       </c>
@@ -1951,8 +2546,14 @@
       <c r="C101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:3">
+      <c r="E101">
+        <v>-1</v>
+      </c>
+      <c r="F101">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
       <c r="A102" t="s">
         <v>100</v>
       </c>
@@ -1962,8 +2563,14 @@
       <c r="C102">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="103" spans="1:3">
+      <c r="E102">
+        <v>-0.5</v>
+      </c>
+      <c r="F102">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
       <c r="A103" t="s">
         <v>101</v>
       </c>
@@ -1973,8 +2580,14 @@
       <c r="C103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:3">
+      <c r="E103">
+        <v>-1</v>
+      </c>
+      <c r="F103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -1984,8 +2597,14 @@
       <c r="C104">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="105" spans="1:3">
+      <c r="E104">
+        <v>-1</v>
+      </c>
+      <c r="F104">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
       <c r="A105" t="s">
         <v>103</v>
       </c>
@@ -1995,8 +2614,14 @@
       <c r="C105">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="106" spans="1:3">
+      <c r="E105">
+        <v>0.5</v>
+      </c>
+      <c r="F105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
       <c r="A106" t="s">
         <v>104</v>
       </c>
@@ -2006,8 +2631,14 @@
       <c r="C106">
         <v>-1</v>
       </c>
-    </row>
-    <row r="107" spans="1:3">
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="F106">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
       <c r="A107" t="s">
         <v>105</v>
       </c>
@@ -2017,8 +2648,14 @@
       <c r="C107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:3">
+      <c r="E107">
+        <v>0.5</v>
+      </c>
+      <c r="F107">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
       <c r="A108" t="s">
         <v>106</v>
       </c>
@@ -2028,8 +2665,14 @@
       <c r="C108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:3">
+      <c r="E108">
+        <v>0.5</v>
+      </c>
+      <c r="F108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
       <c r="A109" t="s">
         <v>107</v>
       </c>
@@ -2039,8 +2682,14 @@
       <c r="C109">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="110" spans="1:3">
+      <c r="E109">
+        <v>-0.5</v>
+      </c>
+      <c r="F109">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
       <c r="A110" t="s">
         <v>108</v>
       </c>
@@ -2050,8 +2699,14 @@
       <c r="C110">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:3">
+      <c r="E110">
+        <v>1</v>
+      </c>
+      <c r="F110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
       <c r="A111" t="s">
         <v>109</v>
       </c>
@@ -2061,8 +2716,14 @@
       <c r="C111">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:3">
+      <c r="E111">
+        <v>-0.5</v>
+      </c>
+      <c r="F111">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
       <c r="A112" t="s">
         <v>110</v>
       </c>
@@ -2072,8 +2733,14 @@
       <c r="C112">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="113" spans="1:3">
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="F112">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
       <c r="A113" t="s">
         <v>111</v>
       </c>
@@ -2083,8 +2750,14 @@
       <c r="C113">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:3">
+      <c r="E113">
+        <v>1</v>
+      </c>
+      <c r="F113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
       <c r="A114" t="s">
         <v>112</v>
       </c>
@@ -2094,8 +2767,14 @@
       <c r="C114">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="115" spans="1:3">
+      <c r="E114">
+        <v>0.5</v>
+      </c>
+      <c r="F114">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
       <c r="A115" t="s">
         <v>113</v>
       </c>
@@ -2105,8 +2784,14 @@
       <c r="C115">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="116" spans="1:3">
+      <c r="E115">
+        <v>-1</v>
+      </c>
+      <c r="F115">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
       <c r="A116" t="s">
         <v>114</v>
       </c>
@@ -2116,8 +2801,14 @@
       <c r="C116">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:3">
+      <c r="E116">
+        <v>-1</v>
+      </c>
+      <c r="F116">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
       <c r="A117" t="s">
         <v>115</v>
       </c>
@@ -2127,8 +2818,14 @@
       <c r="C117">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="118" spans="1:3">
+      <c r="E117">
+        <v>-0.5</v>
+      </c>
+      <c r="F117">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
       <c r="A118" t="s">
         <v>116</v>
       </c>
@@ -2138,8 +2835,14 @@
       <c r="C118">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="119" spans="1:3">
+      <c r="E118">
+        <v>0.5</v>
+      </c>
+      <c r="F118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
       <c r="A119" t="s">
         <v>117</v>
       </c>
@@ -2149,8 +2852,14 @@
       <c r="C119">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="120" spans="1:3">
+      <c r="E119">
+        <v>1</v>
+      </c>
+      <c r="F119">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
       <c r="A120" t="s">
         <v>118</v>
       </c>
@@ -2160,8 +2869,14 @@
       <c r="C120">
         <v>-1</v>
       </c>
-    </row>
-    <row r="121" spans="1:3">
+      <c r="E120">
+        <v>0.5</v>
+      </c>
+      <c r="F120">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
       <c r="A121" t="s">
         <v>119</v>
       </c>
@@ -2171,8 +2886,14 @@
       <c r="C121">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:3">
+      <c r="E121">
+        <v>-1</v>
+      </c>
+      <c r="F121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
       <c r="A122" t="s">
         <v>120</v>
       </c>
@@ -2182,8 +2903,14 @@
       <c r="C122">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="123" spans="1:3">
+      <c r="E122">
+        <v>-1</v>
+      </c>
+      <c r="F122">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
       <c r="A123" t="s">
         <v>121</v>
       </c>
@@ -2193,8 +2920,14 @@
       <c r="C123">
         <v>-1</v>
       </c>
-    </row>
-    <row r="124" spans="1:3">
+      <c r="E123">
+        <v>-1</v>
+      </c>
+      <c r="F123">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
       <c r="A124" t="s">
         <v>122</v>
       </c>
@@ -2204,8 +2937,14 @@
       <c r="C124">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:3">
+      <c r="E124">
+        <v>0</v>
+      </c>
+      <c r="F124">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
       <c r="A125" t="s">
         <v>123</v>
       </c>
@@ -2215,8 +2954,14 @@
       <c r="C125">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:3">
+      <c r="E125">
+        <v>0.5</v>
+      </c>
+      <c r="F125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
       <c r="A126" t="s">
         <v>124</v>
       </c>
@@ -2226,8 +2971,14 @@
       <c r="C126">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:3">
+      <c r="E126">
+        <v>-0.5</v>
+      </c>
+      <c r="F126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
       <c r="A127" t="s">
         <v>125</v>
       </c>
@@ -2237,8 +2988,14 @@
       <c r="C127">
         <v>-1</v>
       </c>
-    </row>
-    <row r="128" spans="1:3">
+      <c r="E127">
+        <v>-1</v>
+      </c>
+      <c r="F127">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
       <c r="A128" s="1" t="s">
         <v>126</v>
       </c>
@@ -2248,8 +3005,14 @@
       <c r="C128">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:3">
+      <c r="E128">
+        <v>0</v>
+      </c>
+      <c r="F128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
       <c r="A129" t="s">
         <v>127</v>
       </c>
@@ -2259,8 +3022,14 @@
       <c r="C129">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:3">
+      <c r="E129">
+        <v>1</v>
+      </c>
+      <c r="F129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
       <c r="A130" t="s">
         <v>128</v>
       </c>
@@ -2270,8 +3039,14 @@
       <c r="C130">
         <v>-1</v>
       </c>
-    </row>
-    <row r="131" spans="1:3">
+      <c r="E130">
+        <v>-0.5</v>
+      </c>
+      <c r="F130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
       <c r="A131" t="s">
         <v>129</v>
       </c>
@@ -2281,8 +3056,14 @@
       <c r="C131">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="132" spans="1:3">
+      <c r="E131">
+        <v>1</v>
+      </c>
+      <c r="F131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
       <c r="A132" t="s">
         <v>130</v>
       </c>
@@ -2292,8 +3073,14 @@
       <c r="C132">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="133" spans="1:3">
+      <c r="E132">
+        <v>0.5</v>
+      </c>
+      <c r="F132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
       <c r="A133" t="s">
         <v>131</v>
       </c>
@@ -2303,8 +3090,14 @@
       <c r="C133">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:3">
+      <c r="E133">
+        <v>0.5</v>
+      </c>
+      <c r="F133">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
       <c r="A134" t="s">
         <v>132</v>
       </c>
@@ -2314,8 +3107,14 @@
       <c r="C134">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="135" spans="1:3">
+      <c r="E134">
+        <v>-1</v>
+      </c>
+      <c r="F134">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
       <c r="A135" t="s">
         <v>133</v>
       </c>
@@ -2325,8 +3124,14 @@
       <c r="C135">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:3">
+      <c r="E135">
+        <v>-1</v>
+      </c>
+      <c r="F135">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
       <c r="A136" t="s">
         <v>134</v>
       </c>
@@ -2336,8 +3141,14 @@
       <c r="C136">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:3">
+      <c r="E136">
+        <v>0.5</v>
+      </c>
+      <c r="F136">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
       <c r="A137" t="s">
         <v>135</v>
       </c>
@@ -2347,8 +3158,14 @@
       <c r="C137">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="138" spans="1:3">
+      <c r="E137">
+        <v>0.5</v>
+      </c>
+      <c r="F137">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
       <c r="A138" t="s">
         <v>136</v>
       </c>
@@ -2358,8 +3175,14 @@
       <c r="C138">
         <v>-1</v>
       </c>
-    </row>
-    <row r="139" spans="1:3">
+      <c r="E138">
+        <v>-1</v>
+      </c>
+      <c r="F138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
       <c r="A139" t="s">
         <v>137</v>
       </c>
@@ -2369,8 +3192,14 @@
       <c r="C139">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="140" spans="1:3">
+      <c r="E139">
+        <v>0</v>
+      </c>
+      <c r="F139">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
       <c r="A140" t="s">
         <v>138</v>
       </c>
@@ -2380,8 +3209,14 @@
       <c r="C140">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="141" spans="1:3">
+      <c r="E140">
+        <v>0</v>
+      </c>
+      <c r="F140">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
       <c r="A141" t="s">
         <v>139</v>
       </c>
@@ -2391,8 +3226,14 @@
       <c r="C141">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="142" spans="1:3">
+      <c r="E141">
+        <v>-0.5</v>
+      </c>
+      <c r="F141">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
       <c r="A142" t="s">
         <v>140</v>
       </c>
@@ -2402,8 +3243,14 @@
       <c r="C142">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="143" spans="1:3">
+      <c r="E142">
+        <v>0.5</v>
+      </c>
+      <c r="F142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
       <c r="A143" t="s">
         <v>141</v>
       </c>
@@ -2413,9 +3260,15 @@
       <c r="C143">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:3">
-      <c r="A144" s="1" t="s">
+      <c r="E143">
+        <v>-0.5</v>
+      </c>
+      <c r="F143">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B144">
@@ -2424,8 +3277,14 @@
       <c r="C144">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="145" spans="1:3">
+      <c r="E144">
+        <v>-0.5</v>
+      </c>
+      <c r="F144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
       <c r="A145" t="s">
         <v>143</v>
       </c>
@@ -2435,8 +3294,14 @@
       <c r="C145">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:3">
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="F145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
       <c r="A146" t="s">
         <v>144</v>
       </c>
@@ -2446,8 +3311,14 @@
       <c r="C146">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:3">
+      <c r="E146">
+        <v>0.5</v>
+      </c>
+      <c r="F146">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
       <c r="A147" t="s">
         <v>145</v>
       </c>
@@ -2457,8 +3328,14 @@
       <c r="C147">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:3">
+      <c r="E147">
+        <v>0.5</v>
+      </c>
+      <c r="F147">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
       <c r="A148" t="s">
         <v>146</v>
       </c>
@@ -2468,8 +3345,14 @@
       <c r="C148">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="149" spans="1:3">
+      <c r="E148">
+        <v>-1</v>
+      </c>
+      <c r="F148">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
       <c r="A149" t="s">
         <v>147</v>
       </c>
@@ -2479,8 +3362,14 @@
       <c r="C149">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="150" spans="1:3">
+      <c r="E149">
+        <v>-0.5</v>
+      </c>
+      <c r="F149">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
       <c r="A150" t="s">
         <v>148</v>
       </c>
@@ -2490,8 +3379,14 @@
       <c r="C150">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="151" spans="1:3">
+      <c r="E150">
+        <v>0.5</v>
+      </c>
+      <c r="F150">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
       <c r="A151" t="s">
         <v>149</v>
       </c>
@@ -2500,6 +3395,12 @@
       </c>
       <c r="C151">
         <v>0</v>
+      </c>
+      <c r="E151">
+        <v>1</v>
+      </c>
+      <c r="F151">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>